<commit_message>
Sends txt to whatsApp contacts via xlsx file
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -21,10 +21,10 @@
     <t>WhatsapNo</t>
   </si>
   <si>
-    <t>Ram</t>
+    <t>Patidev</t>
   </si>
   <si>
-    <t>Rahul</t>
+    <t>Rishabh</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated data provider xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -16,15 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>WhatsapNo</t>
-  </si>
-  <si>
-    <t>Patidev</t>
-  </si>
-  <si>
-    <t>Rishabh</t>
   </si>
 </sst>
 </file>
@@ -380,13 +374,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>